<commit_message>
fix(RNAFUSION orders) Add validation for one sample per case (#2209)(minor)
### Added
- Validation for RNAFUSION orders to only allow one sample per case
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1508.28.rnafusion.xlsx
+++ b/tests/fixtures/orderforms/1508.28.rnafusion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincent.janvid/dev/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5369F30-857B-7A43-960A-0EAF47DA7906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D1CC70-25A6-1243-919D-97DBD7289325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41140" yWindow="3680" windowWidth="36340" windowHeight="22900" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41140" yWindow="-3580" windowWidth="36340" windowHeight="22900" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="information" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="711">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="713">
   <si>
     <t>https://clinical.scilifelab.se/</t>
   </si>
@@ -3148,6 +3148,12 @@
   <si>
     <t>comment</t>
   </si>
+  <si>
+    <t>miprnacase41</t>
+  </si>
+  <si>
+    <t>miprnacase42</t>
+  </si>
 </sst>
 </file>
 
@@ -5159,8 +5165,8 @@
   </sheetPr>
   <dimension ref="A1:AMO395"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="R13" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="AH15" sqref="AH15:AL16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="1" x14ac:dyDescent="0.15"/>
@@ -13946,7 +13952,7 @@
         <v>561</v>
       </c>
       <c r="E16" s="70" t="s">
-        <v>585</v>
+        <v>711</v>
       </c>
       <c r="F16" s="70" t="s">
         <v>243</v>
@@ -15014,7 +15020,7 @@
         <v>561</v>
       </c>
       <c r="E17" s="70" t="s">
-        <v>585</v>
+        <v>712</v>
       </c>
       <c r="F17" s="70" t="s">
         <v>525</v>

</xml_diff>